<commit_message>
updated for jan 31
</commit_message>
<xml_diff>
--- a/excelfiles/MW-NIFTY-50-31-Dec-2025.xlsx
+++ b/excelfiles/MW-NIFTY-50-31-Dec-2025.xlsx
@@ -15,13 +15,14 @@
   <sheets>
     <sheet name="MW-NIFTY-50-31-Dec-2025" sheetId="1" r:id="rId1"/>
     <sheet name="Result" r:id="rId5" sheetId="2"/>
+    <sheet name="Result1" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="124">
   <si>
     <t xml:space="preserve">SYMBOL 
 </t>
@@ -405,6 +406,9 @@
   </si>
   <si>
     <t>DiffFrom52WHigh</t>
+  </si>
+  <si>
+    <t>DiffFrom52WLow</t>
   </si>
 </sst>
 </file>
@@ -4603,4 +4607,1034 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>367.4</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>810.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>45.358024691358025</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>337.7</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>108.79478827361564</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>4276.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>7493.05</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>57.06621469228152</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>3930.1</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>108.80130276583293</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>3210.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>4322.95</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>74.2548491192357</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>2866.6</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>111.97934835693853</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>278.05</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>368.45</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>75.4647849097571</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>194.8</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>142.73613963039014</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>1045.1</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>1314.3</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>79.51761393897893</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>940.05</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>111.17493750332429</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>1620.1</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>2012.2</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>80.5138654209323</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>1302.75</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>124.36000767606984</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>5060.0</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>6232.5</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>81.18732450862414</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>3945.0</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>128.2636248415716</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>264.0</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>324.6</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>81.33086876155267</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>228.0</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>115.78947368421053</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>1617.9</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>1982.8</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>81.59673189429091</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>1307.0</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>123.78729915837796</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>402.7</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>491.0</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>82.01629327902239</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>390.15</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>103.21671152120979</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>264.2</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>322.0</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>82.04968944099377</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <v>247.3</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <v>106.83380509502626</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>2317.0</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>2750.0</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>84.25454545454545</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>2136.0</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>108.47378277153558</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>2239.0</v>
+      </c>
+      <c r="C14" t="n" s="0">
+        <v>2616.5</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>85.57232944773553</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>1967.52</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>113.79808083272343</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B15" t="n" s="0">
+        <v>7039.0</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>8099.5</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>86.90659917278843</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>6001.0</v>
+      </c>
+      <c r="F15" t="n" s="0">
+        <v>117.29711714714215</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B16" t="n" s="0">
+        <v>295.0</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>338.6</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>87.12344949793265</v>
+      </c>
+      <c r="E16" t="n" s="0">
+        <v>198.65</v>
+      </c>
+      <c r="F16" t="n" s="0">
+        <v>148.50239114019632</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B17" t="n" s="0">
+        <v>240.46</v>
+      </c>
+      <c r="C17" t="n" s="0">
+        <v>273.5</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>87.91956124314443</v>
+      </c>
+      <c r="E17" t="n" s="0">
+        <v>205.0</v>
+      </c>
+      <c r="F17" t="n" s="0">
+        <v>117.29756097560977</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B18" t="n" s="0">
+        <v>329.9</v>
+      </c>
+      <c r="C18" t="n" s="0">
+        <v>371.45</v>
+      </c>
+      <c r="D18" t="n" s="0">
+        <v>88.81410687844932</v>
+      </c>
+      <c r="E18" t="n" s="0">
+        <v>292.8</v>
+      </c>
+      <c r="F18" t="n" s="0">
+        <v>112.6707650273224</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="B19" t="n" s="0">
+        <v>986.5</v>
+      </c>
+      <c r="C19" t="n" s="0">
+        <v>1102.5</v>
+      </c>
+      <c r="D19" t="n" s="0">
+        <v>89.47845804988661</v>
+      </c>
+      <c r="E19" t="n" s="0">
+        <v>679.2</v>
+      </c>
+      <c r="F19" t="n" s="0">
+        <v>145.2444051825677</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="B20" t="n" s="0">
+        <v>1343.0</v>
+      </c>
+      <c r="C20" t="n" s="0">
+        <v>1500.0</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>89.53333333333333</v>
+      </c>
+      <c r="E20" t="n" s="0">
+        <v>1186.0</v>
+      </c>
+      <c r="F20" t="n" s="0">
+        <v>113.23777403035413</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="B21" t="n" s="0">
+        <v>1591.0</v>
+      </c>
+      <c r="C21" t="n" s="0">
+        <v>1773.6</v>
+      </c>
+      <c r="D21" t="n" s="0">
+        <v>89.70455570590889</v>
+      </c>
+      <c r="E21" t="n" s="0">
+        <v>1209.4</v>
+      </c>
+      <c r="F21" t="n" s="0">
+        <v>131.55283611708285</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B22" t="n" s="0">
+        <v>11792.0</v>
+      </c>
+      <c r="C22" t="n" s="0">
+        <v>13097.0</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>90.03588608078186</v>
+      </c>
+      <c r="E22" t="n" s="0">
+        <v>10047.85</v>
+      </c>
+      <c r="F22" t="n" s="0">
+        <v>117.3584398652448</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B23" t="n" s="0">
+        <v>1720.0</v>
+      </c>
+      <c r="C23" t="n" s="0">
+        <v>1910.0</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>90.0523560209424</v>
+      </c>
+      <c r="E23" t="n" s="0">
+        <v>1548.0</v>
+      </c>
+      <c r="F23" t="n" s="0">
+        <v>111.11111111111111</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B24" t="n" s="0">
+        <v>1508.1</v>
+      </c>
+      <c r="C24" t="n" s="0">
+        <v>1673.0</v>
+      </c>
+      <c r="D24" t="n" s="0">
+        <v>90.14345487148833</v>
+      </c>
+      <c r="E24" t="n" s="0">
+        <v>1335.0</v>
+      </c>
+      <c r="F24" t="n" s="0">
+        <v>112.96629213483146</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B25" t="n" s="0">
+        <v>1273.0</v>
+      </c>
+      <c r="C25" t="n" s="0">
+        <v>1405.9</v>
+      </c>
+      <c r="D25" t="n" s="0">
+        <v>90.5469805818337</v>
+      </c>
+      <c r="E25" t="n" s="0">
+        <v>1020.0</v>
+      </c>
+      <c r="F25" t="n" s="0">
+        <v>124.80392156862746</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B26" t="n" s="0">
+        <v>749.05</v>
+      </c>
+      <c r="C26" t="n" s="0">
+        <v>820.75</v>
+      </c>
+      <c r="D26" t="n" s="0">
+        <v>91.2640877246421</v>
+      </c>
+      <c r="E26" t="n" s="0">
+        <v>584.3</v>
+      </c>
+      <c r="F26" t="n" s="0">
+        <v>128.19613212390894</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B27" t="n" s="0">
+        <v>399.2</v>
+      </c>
+      <c r="C27" t="n" s="0">
+        <v>436.0</v>
+      </c>
+      <c r="D27" t="n" s="0">
+        <v>91.55963302752292</v>
+      </c>
+      <c r="E27" t="n" s="0">
+        <v>240.25</v>
+      </c>
+      <c r="F27" t="n" s="0">
+        <v>166.16024973985432</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B28" t="n" s="0">
+        <v>2770.2</v>
+      </c>
+      <c r="C28" t="n" s="0">
+        <v>2985.7</v>
+      </c>
+      <c r="D28" t="n" s="0">
+        <v>92.78226211608667</v>
+      </c>
+      <c r="E28" t="n" s="0">
+        <v>2124.75</v>
+      </c>
+      <c r="F28" t="n" s="0">
+        <v>130.37769149311683</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B29" t="n" s="0">
+        <v>2038.0</v>
+      </c>
+      <c r="C29" t="n" s="0">
+        <v>2195.0</v>
+      </c>
+      <c r="D29" t="n" s="0">
+        <v>92.84738041002278</v>
+      </c>
+      <c r="E29" t="n" s="0">
+        <v>1560.0</v>
+      </c>
+      <c r="F29" t="n" s="0">
+        <v>130.64102564102564</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="B30" t="n" s="0">
+        <v>1469.7</v>
+      </c>
+      <c r="C30" t="n" s="0">
+        <v>1549.0</v>
+      </c>
+      <c r="D30" t="n" s="0">
+        <v>94.88056810845707</v>
+      </c>
+      <c r="E30" t="n" s="0">
+        <v>1010.75</v>
+      </c>
+      <c r="F30" t="n" s="0">
+        <v>145.40687608211724</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="B31" t="n" s="0">
+        <v>2833.0</v>
+      </c>
+      <c r="C31" t="n" s="0">
+        <v>2977.8</v>
+      </c>
+      <c r="D31" t="n" s="0">
+        <v>95.13734972127072</v>
+      </c>
+      <c r="E31" t="n" s="0">
+        <v>2276.95</v>
+      </c>
+      <c r="F31" t="n" s="0">
+        <v>124.42082610509675</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B32" t="n" s="0">
+        <v>1165.9</v>
+      </c>
+      <c r="C32" t="n" s="0">
+        <v>1223.9</v>
+      </c>
+      <c r="D32" t="n" s="0">
+        <v>95.2610507394395</v>
+      </c>
+      <c r="E32" t="n" s="0">
+        <v>880.0</v>
+      </c>
+      <c r="F32" t="n" s="0">
+        <v>132.48863636363637</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B33" t="n" s="0">
+        <v>2203.0</v>
+      </c>
+      <c r="C33" t="n" s="0">
+        <v>2301.9</v>
+      </c>
+      <c r="D33" t="n" s="0">
+        <v>95.70354924193057</v>
+      </c>
+      <c r="E33" t="n" s="0">
+        <v>1723.75</v>
+      </c>
+      <c r="F33" t="n" s="0">
+        <v>127.8027556200145</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B34" t="n" s="0">
+        <v>399.45</v>
+      </c>
+      <c r="C34" t="n" s="0">
+        <v>417.25</v>
+      </c>
+      <c r="D34" t="n" s="0">
+        <v>95.73397243858597</v>
+      </c>
+      <c r="E34" t="n" s="0">
+        <v>349.25</v>
+      </c>
+      <c r="F34" t="n" s="0">
+        <v>114.37365783822476</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B35" t="n" s="0">
+        <v>179.93</v>
+      </c>
+      <c r="C35" t="n" s="0">
+        <v>186.94</v>
+      </c>
+      <c r="D35" t="n" s="0">
+        <v>96.25013373274848</v>
+      </c>
+      <c r="E35" t="n" s="0">
+        <v>122.62</v>
+      </c>
+      <c r="F35" t="n" s="0">
+        <v>146.73788941445116</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B36" t="n" s="0">
+        <v>2107.0</v>
+      </c>
+      <c r="C36" t="n" s="0">
+        <v>2174.5</v>
+      </c>
+      <c r="D36" t="n" s="0">
+        <v>96.8958381237066</v>
+      </c>
+      <c r="E36" t="n" s="0">
+        <v>1559.5</v>
+      </c>
+      <c r="F36" t="n" s="0">
+        <v>135.10740621994228</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B37" t="n" s="0">
+        <v>1268.7</v>
+      </c>
+      <c r="C37" t="n" s="0">
+        <v>1304.0</v>
+      </c>
+      <c r="D37" t="n" s="0">
+        <v>97.29294478527608</v>
+      </c>
+      <c r="E37" t="n" s="0">
+        <v>933.5</v>
+      </c>
+      <c r="F37" t="n" s="0">
+        <v>135.90787359400107</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B38" t="n" s="0">
+        <v>992.9</v>
+      </c>
+      <c r="C38" t="n" s="0">
+        <v>1020.5</v>
+      </c>
+      <c r="D38" t="n" s="0">
+        <v>97.29544341009309</v>
+      </c>
+      <c r="E38" t="n" s="0">
+        <v>812.15</v>
+      </c>
+      <c r="F38" t="n" s="0">
+        <v>122.25574093455643</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B39" t="n" s="0">
+        <v>2031.5</v>
+      </c>
+      <c r="C39" t="n" s="0">
+        <v>2086.6</v>
+      </c>
+      <c r="D39" t="n" s="0">
+        <v>97.35934055401131</v>
+      </c>
+      <c r="E39" t="n" s="0">
+        <v>1372.55</v>
+      </c>
+      <c r="F39" t="n" s="0">
+        <v>148.00917999344287</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B40" t="n" s="0">
+        <v>3716.0</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>3795.0</v>
+      </c>
+      <c r="D40" t="n" s="0">
+        <v>97.91831357048747</v>
+      </c>
+      <c r="E40" t="n" s="0">
+        <v>2425.0</v>
+      </c>
+      <c r="F40" t="n" s="0">
+        <v>153.23711340206185</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B41" t="n" s="0">
+        <v>1287.0</v>
+      </c>
+      <c r="C41" t="n" s="0">
+        <v>1311.6</v>
+      </c>
+      <c r="D41" t="n" s="0">
+        <v>98.12442817932296</v>
+      </c>
+      <c r="E41" t="n" s="0">
+        <v>1055.0</v>
+      </c>
+      <c r="F41" t="n" s="0">
+        <v>121.9905213270142</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B42" t="n" s="0">
+        <v>982.4</v>
+      </c>
+      <c r="C42" t="n" s="0">
+        <v>999.0</v>
+      </c>
+      <c r="D42" t="n" s="0">
+        <v>98.33833833833833</v>
+      </c>
+      <c r="E42" t="n" s="0">
+        <v>680.0</v>
+      </c>
+      <c r="F42" t="n" s="0">
+        <v>144.47058823529412</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B43" t="n" s="0">
+        <v>9350.0</v>
+      </c>
+      <c r="C43" t="n" s="0">
+        <v>9490.0</v>
+      </c>
+      <c r="D43" t="n" s="0">
+        <v>98.52476290832455</v>
+      </c>
+      <c r="E43" t="n" s="0">
+        <v>7089.35</v>
+      </c>
+      <c r="F43" t="n" s="0">
+        <v>131.88797280427684</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B44" t="n" s="0">
+        <v>4083.0</v>
+      </c>
+      <c r="C44" t="n" s="0">
+        <v>4140.0</v>
+      </c>
+      <c r="D44" t="n" s="0">
+        <v>98.62318840579711</v>
+      </c>
+      <c r="E44" t="n" s="0">
+        <v>2965.3</v>
+      </c>
+      <c r="F44" t="n" s="0">
+        <v>137.69264492631436</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="B45" t="n" s="0">
+        <v>1190.1</v>
+      </c>
+      <c r="C45" t="n" s="0">
+        <v>1202.8</v>
+      </c>
+      <c r="D45" t="n" s="0">
+        <v>98.94413036248753</v>
+      </c>
+      <c r="E45" t="n" s="0">
+        <v>893.1</v>
+      </c>
+      <c r="F45" t="n" s="0">
+        <v>133.25495465233453</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B46" t="n" s="0">
+        <v>7314.0</v>
+      </c>
+      <c r="C46" t="n" s="0">
+        <v>7374.5</v>
+      </c>
+      <c r="D46" t="n" s="0">
+        <v>99.17960539697606</v>
+      </c>
+      <c r="E46" t="n" s="0">
+        <v>4646.0</v>
+      </c>
+      <c r="F46" t="n" s="0">
+        <v>157.4257425742574</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B47" t="n" s="0">
+        <v>1569.0</v>
+      </c>
+      <c r="C47" t="n" s="0">
+        <v>1581.3</v>
+      </c>
+      <c r="D47" t="n" s="0">
+        <v>99.22215898311516</v>
+      </c>
+      <c r="E47" t="n" s="0">
+        <v>1114.85</v>
+      </c>
+      <c r="F47" t="n" s="0">
+        <v>140.73642194017134</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B48" t="n" s="0">
+        <v>16688.0</v>
+      </c>
+      <c r="C48" t="n" s="0">
+        <v>16818.0</v>
+      </c>
+      <c r="D48" t="n" s="0">
+        <v>99.2270186704721</v>
+      </c>
+      <c r="E48" t="n" s="0">
+        <v>10750.1</v>
+      </c>
+      <c r="F48" t="n" s="0">
+        <v>155.23576524869534</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B49" t="n" s="0">
+        <v>886.0</v>
+      </c>
+      <c r="C49" t="n" s="0">
+        <v>890.0</v>
+      </c>
+      <c r="D49" t="n" s="0">
+        <v>99.5505617977528</v>
+      </c>
+      <c r="E49" t="n" s="0">
+        <v>546.45</v>
+      </c>
+      <c r="F49" t="n" s="0">
+        <v>162.13743251898617</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B50" t="n" s="0">
+        <v>4048.0</v>
+      </c>
+      <c r="C50" t="n" s="0">
+        <v>4061.9</v>
+      </c>
+      <c r="D50" t="n" s="0">
+        <v>99.65779561289052</v>
+      </c>
+      <c r="E50" t="n" s="0">
+        <v>2925.0</v>
+      </c>
+      <c r="F50" t="n" s="0">
+        <v>138.39316239316238</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B51" t="n" s="0">
+        <v>996.8</v>
+      </c>
+      <c r="C51" t="n" s="0">
+        <v>1000.2</v>
+      </c>
+      <c r="D51" t="n" s="0">
+        <v>99.66006798640271</v>
+      </c>
+      <c r="E51" t="n" s="0">
+        <v>493.35</v>
+      </c>
+      <c r="F51" t="n" s="0">
+        <v>202.04722813418462</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>